<commit_message>
add pig breeder data
</commit_message>
<xml_diff>
--- a/storage/database/choice.xlsx
+++ b/storage/database/choice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspaces\LaravelWS\PigFarm\storage\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2D8E91-8101-4BBA-8C61-3D8A950AD8CF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7616BA39-3A88-43F2-A5AF-58F47BFBD010}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27636" windowHeight="14004" xr2:uid="{9961011E-DC10-4E76-B192-29200FDB07B8}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -203,6 +203,30 @@
   </si>
   <si>
     <t>BREED_004</t>
+  </si>
+  <si>
+    <t>BREEDERSTATUS</t>
+  </si>
+  <si>
+    <t>สถานะการผสมพันธุ์</t>
+  </si>
+  <si>
+    <t>BREEDERSTATUS_001</t>
+  </si>
+  <si>
+    <t>BREEDERSTATUS_002</t>
+  </si>
+  <si>
+    <t>ปกติ</t>
+  </si>
+  <si>
+    <t>สำเร็จ</t>
+  </si>
+  <si>
+    <t>BREEDERSTATUS_003</t>
+  </si>
+  <si>
+    <t>ล้มเหลว</t>
   </si>
 </sst>
 </file>
@@ -557,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2820448-9907-429D-8FAD-8BDDCA1DD31A}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,6 +1021,59 @@
         <v>53</v>
       </c>
     </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>